<commit_message>
Marot et al 2022 hook update
</commit_message>
<xml_diff>
--- a/data/primary_studies/Marot_et_al_2020/original/Marot_et_al_2020_methods.xlsx
+++ b/data/primary_studies/Marot_et_al_2020/original/Marot_et_al_2020_methods.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henry/Documents/CCN_GitHub/CCRCN-Data-Library/data/primary_studies/Marot_et_al_2020/original/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henry/Documents/CCN GitHub/CCRCN-Data-Library/data/primary_studies/Marot_et_al_2020/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2537EE7-A76D-9148-A2C6-7EEB51D03997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E15463-F8B2-E546-8421-DDB14BF7FCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15740" windowHeight="16160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="133">
   <si>
     <t>column_name</t>
   </si>
@@ -341,9 +341,6 @@
     <t>time approximate</t>
   </si>
   <si>
-    <t>also 110C for 6h</t>
-  </si>
-  <si>
     <t>surface sample</t>
   </si>
   <si>
@@ -365,49 +362,64 @@
     <t>gamma</t>
   </si>
   <si>
-    <t>roots and rhizomes included?</t>
-  </si>
-  <si>
     <t>selected samples</t>
   </si>
   <si>
     <t>AMS</t>
   </si>
   <si>
-    <t>vibracore_alpha</t>
-  </si>
-  <si>
-    <t>vibracore_gamma</t>
-  </si>
-  <si>
-    <t>pushcore_alpha</t>
-  </si>
-  <si>
-    <t>pushcore_gamma</t>
-  </si>
-  <si>
-    <t>shovelcore_alpha</t>
-  </si>
-  <si>
-    <t>shovelcore_gamma</t>
-  </si>
-  <si>
-    <t>russiancorer_gamma</t>
-  </si>
-  <si>
-    <t>russiancorer_alpha</t>
-  </si>
-  <si>
-    <t>surfacesample_alpha</t>
-  </si>
-  <si>
-    <t>surfacesample_gamma</t>
-  </si>
-  <si>
-    <t>russian core</t>
-  </si>
-  <si>
     <t>YBP</t>
+  </si>
+  <si>
+    <t>russian corer</t>
+  </si>
+  <si>
+    <t>push_core_no_spectroscopy</t>
+  </si>
+  <si>
+    <t>vibracore_alpha_spectroscopy</t>
+  </si>
+  <si>
+    <t>vibracore_gamma_spectroscopy</t>
+  </si>
+  <si>
+    <t>push_core_alpha_spectroscopy</t>
+  </si>
+  <si>
+    <t>push_core_gamma_spectroscopy</t>
+  </si>
+  <si>
+    <t>surface_sample_gamma_spectroscopy</t>
+  </si>
+  <si>
+    <t>surface_sample_alpha_spectroscopy</t>
+  </si>
+  <si>
+    <t>russian_corer_gamma_spectroscopy</t>
+  </si>
+  <si>
+    <t>russian_corer_alpha_spectroscopy</t>
+  </si>
+  <si>
+    <t>shovel_corer_gamma_spectroscopy</t>
+  </si>
+  <si>
+    <t>shovel_corer_alpha_spectroscopy</t>
+  </si>
+  <si>
+    <t>vibracore_no_spectroscopy</t>
+  </si>
+  <si>
+    <t>shovel_corer_no_spectroscopy</t>
+  </si>
+  <si>
+    <t>russian_corer_no_spectroscopy</t>
+  </si>
+  <si>
+    <t>surface_sample_no_spectroscopy</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1403,16 +1415,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG10" sqref="AG10"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
@@ -1546,14 +1558,11 @@
         <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
         <v>99</v>
       </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
       <c r="E2" t="s">
         <v>102</v>
       </c>
@@ -1578,38 +1587,35 @@
       <c r="N2">
         <v>6</v>
       </c>
-      <c r="Q2" t="s">
-        <v>106</v>
-      </c>
       <c r="R2" t="s">
+        <v>107</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
         <v>108</v>
       </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" t="s">
         <v>109</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>111</v>
       </c>
-      <c r="V2" t="s">
-        <v>110</v>
-      </c>
-      <c r="X2" t="s">
-        <v>112</v>
-      </c>
       <c r="Y2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE2" t="s">
         <v>115</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
@@ -1617,14 +1623,11 @@
         <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>99</v>
       </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
       <c r="E3" t="s">
         <v>102</v>
       </c>
@@ -1649,38 +1652,35 @@
       <c r="N3">
         <v>6</v>
       </c>
-      <c r="Q3" t="s">
-        <v>106</v>
-      </c>
       <c r="R3" t="s">
+        <v>107</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
         <v>108</v>
       </c>
-      <c r="S3" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>110</v>
+      </c>
+      <c r="V3" t="s">
         <v>109</v>
       </c>
-      <c r="U3" t="s">
-        <v>111</v>
-      </c>
-      <c r="V3" t="s">
-        <v>110</v>
-      </c>
       <c r="X3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB3" t="s">
         <v>113</v>
       </c>
-      <c r="Y3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE3" t="s">
         <v>115</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
@@ -1688,13 +1688,10 @@
         <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
         <v>102</v>
@@ -1720,38 +1717,35 @@
       <c r="N4">
         <v>6</v>
       </c>
-      <c r="Q4" t="s">
-        <v>106</v>
-      </c>
       <c r="R4" t="s">
+        <v>107</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
         <v>108</v>
       </c>
-      <c r="S4" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
+        <v>110</v>
+      </c>
+      <c r="V4" t="s">
         <v>109</v>
       </c>
-      <c r="U4" t="s">
-        <v>111</v>
-      </c>
-      <c r="V4" t="s">
-        <v>110</v>
-      </c>
       <c r="X4" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="Y4" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="AB4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE4" t="s">
         <v>115</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
@@ -1764,9 +1758,6 @@
       <c r="C5" t="s">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
-        <v>114</v>
-      </c>
       <c r="E5" t="s">
         <v>102</v>
       </c>
@@ -1791,38 +1782,35 @@
       <c r="N5">
         <v>6</v>
       </c>
-      <c r="Q5" t="s">
-        <v>106</v>
-      </c>
       <c r="R5" t="s">
+        <v>107</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
         <v>108</v>
       </c>
-      <c r="S5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
+        <v>110</v>
+      </c>
+      <c r="V5" t="s">
         <v>109</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>111</v>
       </c>
-      <c r="V5" t="s">
-        <v>110</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB5" t="s">
         <v>113</v>
       </c>
-      <c r="Y5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE5" t="s">
         <v>115</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
@@ -1833,10 +1821,7 @@
         <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
         <v>102</v>
@@ -1845,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6">
         <v>60</v>
@@ -1862,23 +1847,20 @@
       <c r="N6">
         <v>6</v>
       </c>
-      <c r="Q6" t="s">
-        <v>106</v>
-      </c>
       <c r="R6" t="s">
+        <v>107</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
         <v>108</v>
       </c>
-      <c r="S6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
+        <v>110</v>
+      </c>
+      <c r="V6" t="s">
         <v>109</v>
-      </c>
-      <c r="U6" t="s">
-        <v>111</v>
-      </c>
-      <c r="V6" t="s">
-        <v>110</v>
       </c>
       <c r="X6" t="s">
         <v>112</v>
@@ -1887,13 +1869,13 @@
         <v>112</v>
       </c>
       <c r="AB6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE6" t="s">
         <v>115</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
@@ -1901,13 +1883,10 @@
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
         <v>102</v>
@@ -1916,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H7">
         <v>60</v>
@@ -1933,38 +1912,35 @@
       <c r="N7">
         <v>6</v>
       </c>
-      <c r="Q7" t="s">
-        <v>106</v>
-      </c>
       <c r="R7" t="s">
+        <v>107</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
         <v>108</v>
       </c>
-      <c r="S7" t="b">
-        <v>1</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
+        <v>110</v>
+      </c>
+      <c r="V7" t="s">
         <v>109</v>
       </c>
-      <c r="U7" t="s">
-        <v>111</v>
-      </c>
-      <c r="V7" t="s">
-        <v>110</v>
-      </c>
       <c r="X7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB7" t="s">
         <v>113</v>
       </c>
-      <c r="Y7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE7" t="s">
         <v>115</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
@@ -1972,13 +1948,10 @@
         <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
         <v>102</v>
@@ -2004,38 +1977,35 @@
       <c r="N8">
         <v>6</v>
       </c>
-      <c r="Q8" t="s">
-        <v>106</v>
-      </c>
       <c r="R8" t="s">
+        <v>107</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
         <v>108</v>
       </c>
-      <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
+        <v>110</v>
+      </c>
+      <c r="V8" t="s">
         <v>109</v>
       </c>
-      <c r="U8" t="s">
+      <c r="X8" t="s">
         <v>111</v>
       </c>
-      <c r="V8" t="s">
-        <v>110</v>
-      </c>
-      <c r="X8" t="s">
-        <v>112</v>
-      </c>
       <c r="Y8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE8" t="s">
         <v>115</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
@@ -2043,13 +2013,10 @@
         <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
         <v>102</v>
@@ -2075,38 +2042,35 @@
       <c r="N9">
         <v>6</v>
       </c>
-      <c r="Q9" t="s">
-        <v>106</v>
-      </c>
       <c r="R9" t="s">
+        <v>107</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
         <v>108</v>
       </c>
-      <c r="S9" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
+        <v>110</v>
+      </c>
+      <c r="V9" t="s">
         <v>109</v>
       </c>
-      <c r="U9" t="s">
-        <v>111</v>
-      </c>
-      <c r="V9" t="s">
-        <v>110</v>
-      </c>
       <c r="X9" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB9" t="s">
         <v>113</v>
       </c>
-      <c r="Y9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE9" t="s">
         <v>115</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
@@ -2114,13 +2078,10 @@
         <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
         <v>102</v>
@@ -2146,38 +2107,35 @@
       <c r="N10">
         <v>6</v>
       </c>
-      <c r="Q10" t="s">
-        <v>106</v>
-      </c>
       <c r="R10" t="s">
+        <v>107</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10" t="s">
         <v>108</v>
       </c>
-      <c r="S10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
+        <v>110</v>
+      </c>
+      <c r="V10" t="s">
         <v>109</v>
       </c>
-      <c r="U10" t="s">
-        <v>111</v>
-      </c>
-      <c r="V10" t="s">
-        <v>110</v>
-      </c>
       <c r="X10" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="Y10" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="AB10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE10" t="s">
         <v>115</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
@@ -2185,13 +2143,10 @@
         <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E11" t="s">
         <v>102</v>
@@ -2217,38 +2172,360 @@
       <c r="N11">
         <v>6</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
+        <v>107</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>108</v>
+      </c>
+      <c r="U11" t="s">
+        <v>110</v>
+      </c>
+      <c r="V11" t="s">
+        <v>109</v>
+      </c>
+      <c r="X11" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12">
+        <v>60</v>
+      </c>
+      <c r="I12">
+        <v>48</v>
+      </c>
+      <c r="L12" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12">
+        <v>550</v>
+      </c>
+      <c r="N12">
+        <v>6</v>
+      </c>
+      <c r="R12" t="s">
+        <v>107</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12" t="s">
+        <v>108</v>
+      </c>
+      <c r="U12" t="s">
+        <v>110</v>
+      </c>
+      <c r="V12" t="s">
+        <v>109</v>
+      </c>
+      <c r="X12" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
+      </c>
+      <c r="I13">
+        <v>48</v>
+      </c>
+      <c r="L13" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13">
+        <v>550</v>
+      </c>
+      <c r="N13">
+        <v>6</v>
+      </c>
+      <c r="R13" t="s">
+        <v>107</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>108</v>
+      </c>
+      <c r="U13" t="s">
+        <v>110</v>
+      </c>
+      <c r="V13" t="s">
+        <v>109</v>
+      </c>
+      <c r="X13" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
         <v>106</v>
       </c>
-      <c r="R11" t="s">
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14">
+        <v>60</v>
+      </c>
+      <c r="I14">
+        <v>48</v>
+      </c>
+      <c r="L14" t="s">
+        <v>105</v>
+      </c>
+      <c r="M14">
+        <v>550</v>
+      </c>
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="R14" t="s">
+        <v>107</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
         <v>108</v>
       </c>
-      <c r="S11" t="b">
-        <v>1</v>
-      </c>
-      <c r="T11" t="s">
+      <c r="U14" t="s">
+        <v>110</v>
+      </c>
+      <c r="V14" t="s">
         <v>109</v>
       </c>
-      <c r="U11" t="s">
+      <c r="X14" t="s">
         <v>111</v>
       </c>
-      <c r="V11" t="s">
+      <c r="Y14" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15">
+        <v>60</v>
+      </c>
+      <c r="I15">
+        <v>48</v>
+      </c>
+      <c r="L15" t="s">
+        <v>105</v>
+      </c>
+      <c r="M15">
+        <v>550</v>
+      </c>
+      <c r="N15">
+        <v>6</v>
+      </c>
+      <c r="R15" t="s">
+        <v>107</v>
+      </c>
+      <c r="S15" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15" t="s">
+        <v>108</v>
+      </c>
+      <c r="U15" t="s">
         <v>110</v>
       </c>
-      <c r="X11" t="s">
+      <c r="V15" t="s">
+        <v>109</v>
+      </c>
+      <c r="X15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB15" t="s">
         <v>113</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AC15" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="I16">
+        <v>48</v>
+      </c>
+      <c r="L16" t="s">
+        <v>105</v>
+      </c>
+      <c r="M16">
+        <v>550</v>
+      </c>
+      <c r="N16">
+        <v>6</v>
+      </c>
+      <c r="R16" t="s">
+        <v>107</v>
+      </c>
+      <c r="S16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16" t="s">
+        <v>108</v>
+      </c>
+      <c r="U16" t="s">
+        <v>110</v>
+      </c>
+      <c r="V16" t="s">
+        <v>109</v>
+      </c>
+      <c r="X16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB16" t="s">
         <v>113</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE16" t="s">
         <v>115</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>